<commit_message>
second to last changes hopefully
</commit_message>
<xml_diff>
--- a/Commissions_BejaouiS_periode_saisie.xlsx
+++ b/Commissions_BejaouiS_periode_saisie.xlsx
@@ -670,21 +670,6 @@
       <c r="A8" t="n">
         <v>2019</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
       <c r="G8" t="n">
         <v>1511826</v>
       </c>
@@ -713,21 +698,6 @@
       <c r="A9" t="n">
         <v>2020</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
       <c r="G9" t="n">
         <v>726578</v>
       </c>
@@ -756,21 +726,6 @@
       <c r="A10" t="n">
         <v>2021</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
       <c r="G10" t="n">
         <v>266544</v>
       </c>
@@ -799,21 +754,6 @@
       <c r="A11" t="n">
         <v>2022</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
@@ -842,21 +782,6 @@
       <c r="A12" t="n">
         <v>2023</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
@@ -885,21 +810,6 @@
       <c r="A13" t="n">
         <v>2024</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
@@ -928,21 +838,6 @@
       <c r="A14" t="n">
         <v>2025</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
@@ -971,21 +866,6 @@
       <c r="A15" t="inlineStr">
         <is>
           <t>Total</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan%</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan%</t>
         </is>
       </c>
       <c r="G15" t="n">

</xml_diff>